<commit_message>
Moved more tests (#227)
</commit_message>
<xml_diff>
--- a/zigar-compiler/test/integeration/test-matrix.xlsx
+++ b/zigar-compiler/test/integeration/test-matrix.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Type handling" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Console" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t xml:space="preserve">Contexts</t>
   </si>
@@ -175,7 +176,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +193,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
   </fills>
@@ -243,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,7 +271,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -334,7 +345,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -355,8 +366,8 @@
   </sheetPr>
   <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -419,7 +430,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -498,10 +509,16 @@
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
@@ -517,23 +534,35 @@
       <c r="L3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="O3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="5"/>
+      <c r="Q3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="T3" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -719,7 +748,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -826,7 +855,7 @@
       <c r="Y13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -853,7 +882,7 @@
       <c r="Y14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -892,4 +921,27 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>